<commit_message>
Ver.6 : Add test pads / NNC and SHARP SSR both support / mode jumper
</commit_message>
<xml_diff>
--- a/KiCad/ESP32DUALDIALBOM.xlsx
+++ b/KiCad/ESP32DUALDIALBOM.xlsx
@@ -190,6 +190,7 @@
       <sz val="10"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -210,6 +211,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -218,15 +220,16 @@
       <color rgb="FFFF0000"/>
       <name val="Noto Sans CJK JP"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
-      <shadow val="true"/>
       <sz val="18"/>
       <color rgb="FFFF0000"/>
       <name val="Noto Serif CJK JP"/>
@@ -275,16 +278,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -319,9 +318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>281520</xdr:colOff>
+      <xdr:colOff>281160</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>8280</xdr:rowOff>
+      <xdr:rowOff>7920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -330,13 +329,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="39768" t="20710" r="32334" b="6570"/>
+        <a:srcRect l="39773" t="20714" r="32339" b="6570"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10292760" y="1710720"/>
-          <a:ext cx="2886120" cy="4104360"/>
+          <a:ext cx="2890800" cy="4104000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -368,8 +367,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4857120" y="244080"/>
-          <a:ext cx="5852160" cy="1964880"/>
+          <a:off x="4857840" y="244080"/>
+          <a:ext cx="5852520" cy="1964880"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -400,9 +399,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2267280</xdr:colOff>
+      <xdr:colOff>2266920</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>64440</xdr:rowOff>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -415,8 +414,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="506520" y="3117600"/>
-          <a:ext cx="5353920" cy="2916360"/>
+          <a:off x="507240" y="3117600"/>
+          <a:ext cx="5353560" cy="2916000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -437,9 +436,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>612720</xdr:colOff>
+      <xdr:colOff>612360</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -452,8 +451,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12930480" y="6990480"/>
-          <a:ext cx="12771720" cy="6951600"/>
+          <a:off x="12935520" y="6990480"/>
+          <a:ext cx="12790440" cy="6951240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -474,9 +473,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>677520</xdr:colOff>
+      <xdr:colOff>677160</xdr:colOff>
       <xdr:row>83</xdr:row>
-      <xdr:rowOff>40680</xdr:rowOff>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -490,7 +489,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6966360"/>
-          <a:ext cx="12762000" cy="6951600"/>
+          <a:ext cx="12765600" cy="6951240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -511,19 +510,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>886320</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>48960</xdr:rowOff>
+      <xdr:colOff>885960</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>115560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="899640" y="3600720"/>
-          <a:ext cx="204840" cy="349560"/>
+          <a:off x="900360" y="3600720"/>
+          <a:ext cx="204480" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -533,11 +532,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -564,19 +574,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>648000</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:colOff>647640</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>213480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4036320" y="4674240"/>
-          <a:ext cx="204840" cy="349560"/>
+          <a:off x="4037040" y="4674240"/>
+          <a:ext cx="204480" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -586,11 +596,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -617,19 +638,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1517760</xdr:colOff>
+      <xdr:colOff>1517400</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>78120</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2381760" y="4746600"/>
-          <a:ext cx="295200" cy="325440"/>
+          <a:off x="2383200" y="4746600"/>
+          <a:ext cx="294840" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -639,11 +660,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -670,19 +702,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>377280</xdr:colOff>
+      <xdr:colOff>376920</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>65520</xdr:rowOff>
+      <xdr:rowOff>10080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="8" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3765600" y="3332880"/>
-          <a:ext cx="204840" cy="308880"/>
+          <a:off x="3766320" y="3332880"/>
+          <a:ext cx="204480" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -692,11 +724,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -723,19 +766,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1641240</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>1640880</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>25920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4840560" y="3348720"/>
-          <a:ext cx="393840" cy="414360"/>
+          <a:off x="4841280" y="3348720"/>
+          <a:ext cx="393480" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -745,11 +788,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -776,19 +830,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1870920</xdr:colOff>
+      <xdr:colOff>1870560</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>138240</xdr:rowOff>
+      <xdr:rowOff>17640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="10" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2726640" y="3340440"/>
-          <a:ext cx="303480" cy="374040"/>
+          <a:off x="2728080" y="3340440"/>
+          <a:ext cx="303120" cy="253440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -798,11 +852,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0">
           <a:spAutoFit/>
         </a:bodyPr>
         <a:p>
+          <a:pPr>
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+          </a:pPr>
           <a:r>
             <a:rPr b="1" lang="en-US" sz="1800" spc="-1" strike="noStrike">
               <a:solidFill>
@@ -820,6 +885,393 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1035000</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>16560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>40680</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>40320</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8435880" y="12268080"/>
+          <a:ext cx="377640" cy="186480"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>583200</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>81000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>993960</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7984080" y="12332520"/>
+          <a:ext cx="410760" cy="8280"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1050120</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>26280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1166400</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>24480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8451000" y="12277800"/>
+          <a:ext cx="116280" cy="160920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>901800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>28080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1036800</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>105480</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8302680" y="11629440"/>
+          <a:ext cx="135000" cy="77400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>897480</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>54720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1032480</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>132120</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8298360" y="11818440"/>
+          <a:ext cx="135000" cy="77400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200880</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>28440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>335880</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>105840</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8973720" y="11467080"/>
+          <a:ext cx="135000" cy="77400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>183600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>79200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>241560</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>13680</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8956440" y="11192760"/>
+          <a:ext cx="57960" cy="259560"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1032120</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>96480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>36000</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>48240</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8433000" y="11372760"/>
+          <a:ext cx="375840" cy="276840"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1040040</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>102960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>43920</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>54720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Line 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8440920" y="11541600"/>
+          <a:ext cx="375840" cy="276840"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="36000">
+          <a:solidFill>
+            <a:srgbClr val="ff0000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:tailEnd len="med" type="triangle" w="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -830,19 +1282,19 @@
   </sheetPr>
   <dimension ref="A1:AMJ41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D52" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G72" activeCellId="0" sqref="G72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1075,26 +1527,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="n">
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="AMI13" s="0"/>
@@ -1216,13 +1668,13 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="3"/>
+      <c r="F30" s="2"/>
     </row>
     <row r="41" customFormat="false" ht="33.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="4" t="s">
+      <c r="C41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="L41" s="4" t="s">
+      <c r="L41" s="3" t="s">
         <v>51</v>
       </c>
     </row>

</xml_diff>